<commit_message>
added graph generator ipynb
</commit_message>
<xml_diff>
--- a/AgImpacts_Raw_Data.xlsx
+++ b/AgImpacts_Raw_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anush\Documents\MIT\TerraELO\WebApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A65A95-7A2E-41CC-BA62-F3A9FD5E7BC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6C61E5-12B6-4C28-910F-BAB3D0F8DEAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16780" windowHeight="5300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9734" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9734" uniqueCount="909">
   <si>
     <t>Variable Name</t>
   </si>
@@ -3476,9 +3476,6 @@
   </si>
   <si>
     <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Victoria state, Queensland state, Western Australia state and Tasmania</t>
   </si>
   <si>
     <t>Sydney, New South Wales state</t>
@@ -4876,9 +4873,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CZ687"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A538" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G495" sqref="G495:H540"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H540" sqref="E495:H540"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -55852,7 +55849,7 @@
       </c>
       <c r="Q360" s="19"/>
     </row>
-    <row r="361" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="361" spans="1:104" outlineLevel="1">
       <c r="B361" s="50" t="s">
         <v>487</v>
       </c>
@@ -55904,7 +55901,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="362" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="362" spans="1:104" outlineLevel="1">
       <c r="B362" s="50" t="s">
         <v>492</v>
       </c>
@@ -55958,7 +55955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="363" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="363" spans="1:104" outlineLevel="1">
       <c r="B363" s="50" t="s">
         <v>496</v>
       </c>
@@ -56012,7 +56009,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="364" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="364" spans="1:104" outlineLevel="1">
       <c r="B364" s="50" t="s">
         <v>501</v>
       </c>
@@ -56066,7 +56063,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="365" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="365" spans="1:104" outlineLevel="1">
       <c r="B365" s="50" t="s">
         <v>502</v>
       </c>
@@ -56120,7 +56117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="366" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="366" spans="1:104" outlineLevel="1">
       <c r="B366" s="50" t="s">
         <v>504</v>
       </c>
@@ -56174,7 +56171,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="367" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="367" spans="1:104" outlineLevel="1">
       <c r="B367" s="50" t="s">
         <v>505</v>
       </c>
@@ -56228,7 +56225,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="368" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="368" spans="1:104" outlineLevel="1">
       <c r="B368" s="50" t="s">
         <v>505</v>
       </c>
@@ -56282,7 +56279,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="369" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="369" spans="2:101" outlineLevel="1">
       <c r="B369" s="50" t="s">
         <v>505</v>
       </c>
@@ -56336,7 +56333,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="370" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="370" spans="2:101" outlineLevel="1">
       <c r="B370" s="50" t="s">
         <v>505</v>
       </c>
@@ -56390,7 +56387,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="371" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="371" spans="2:101" outlineLevel="1">
       <c r="B371" s="50" t="s">
         <v>508</v>
       </c>
@@ -56444,7 +56441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="372" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="372" spans="2:101" outlineLevel="1">
       <c r="B372" s="50" t="s">
         <v>509</v>
       </c>
@@ -56498,7 +56495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="373" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="373" spans="2:101" outlineLevel="1">
       <c r="B373" s="50" t="s">
         <v>509</v>
       </c>
@@ -56552,7 +56549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="374" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="374" spans="2:101" outlineLevel="1">
       <c r="B374" s="50" t="s">
         <v>509</v>
       </c>
@@ -56606,7 +56603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="375" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="375" spans="2:101" outlineLevel="1">
       <c r="B375" s="50" t="s">
         <v>509</v>
       </c>
@@ -56660,7 +56657,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="376" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="376" spans="2:101" outlineLevel="1">
       <c r="B376" s="50" t="s">
         <v>509</v>
       </c>
@@ -56716,7 +56713,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="377" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="377" spans="2:101" outlineLevel="1">
       <c r="B377" s="50" t="s">
         <v>509</v>
       </c>
@@ -56770,7 +56767,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="378" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="378" spans="2:101" outlineLevel="1">
       <c r="B378" s="50" t="s">
         <v>511</v>
       </c>
@@ -56822,7 +56819,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="379" spans="2:101" ht="24.75" hidden="1" customHeight="1" outlineLevel="1">
+    <row r="379" spans="2:101" ht="24.75" customHeight="1" outlineLevel="1">
       <c r="B379" s="50" t="s">
         <v>514</v>
       </c>
@@ -56868,7 +56865,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="380" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="380" spans="2:101" outlineLevel="1">
       <c r="B380" s="50" t="s">
         <v>517</v>
       </c>
@@ -56914,7 +56911,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="381" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="381" spans="2:101" outlineLevel="1">
       <c r="B381" s="50" t="s">
         <v>518</v>
       </c>
@@ -56964,7 +56961,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="382" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="382" spans="2:101" outlineLevel="1">
       <c r="B382" s="50" t="s">
         <v>518</v>
       </c>
@@ -57014,7 +57011,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="383" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="383" spans="2:101" outlineLevel="1">
       <c r="B383" s="50" t="s">
         <v>518</v>
       </c>
@@ -57064,7 +57061,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="384" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="384" spans="2:101" outlineLevel="1">
       <c r="B384" s="50" t="s">
         <v>519</v>
       </c>
@@ -57118,7 +57115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="385" spans="1:17" hidden="1" outlineLevel="1">
+    <row r="385" spans="1:17" outlineLevel="1">
       <c r="B385" s="50" t="s">
         <v>521</v>
       </c>
@@ -57147,7 +57144,7 @@
         <v>0.36480000000000001</v>
       </c>
     </row>
-    <row r="386" spans="1:17" ht="29" hidden="1" outlineLevel="1">
+    <row r="386" spans="1:17" ht="29" outlineLevel="1">
       <c r="B386" s="50" t="s">
         <v>521</v>
       </c>
@@ -57176,7 +57173,7 @@
         <v>0.32640000000000002</v>
       </c>
     </row>
-    <row r="387" spans="1:17" s="18" customFormat="1" collapsed="1">
+    <row r="387" spans="1:17" s="18" customFormat="1">
       <c r="A387" s="18">
         <v>6</v>
       </c>
@@ -62110,7 +62107,7 @@
         <v>734</v>
       </c>
       <c r="E495" s="105" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="F495" s="105" t="s">
         <v>162</v>
@@ -62157,7 +62154,7 @@
         <v>734</v>
       </c>
       <c r="E496" s="105" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F496" s="105" t="s">
         <v>162</v>
@@ -62255,7 +62252,7 @@
         <v>734</v>
       </c>
       <c r="E498" s="105" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F498" s="105" t="s">
         <v>162</v>
@@ -62351,7 +62348,7 @@
         <v>734</v>
       </c>
       <c r="E500" s="105" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="F500" s="105" t="s">
         <v>172</v>
@@ -62449,7 +62446,7 @@
         <v>734</v>
       </c>
       <c r="E502" s="105" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="F502" s="106" t="s">
         <v>172</v>
@@ -62731,7 +62728,7 @@
         <v>751</v>
       </c>
       <c r="E508" s="105" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="F508" s="105" t="s">
         <v>241</v>
@@ -63689,7 +63686,7 @@
         <v>734</v>
       </c>
       <c r="E528" s="105" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F528" s="105" t="s">
         <v>312</v>
@@ -63736,7 +63733,7 @@
         <v>734</v>
       </c>
       <c r="E529" s="105" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="F529" s="105" t="s">
         <v>526</v>
@@ -64255,7 +64252,7 @@
         <v>734</v>
       </c>
       <c r="E540" s="105" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="F540" s="105" t="s">
         <v>485</v>

</xml_diff>

<commit_message>
roundwood 393-394 (latvia) GHG is n/a
</commit_message>
<xml_diff>
--- a/AgImpacts_Raw_Data.xlsx
+++ b/AgImpacts_Raw_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anush\Documents\MIT\TerraELO\WebApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CE1981-31CB-4464-9EB0-C23ABC52BCEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52BB761-9734-42D5-BF3E-DC51BBF6A435}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16780" windowHeight="5300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4899,8 +4899,8 @@
   <dimension ref="A1:CZ692"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B156" sqref="B156"/>
+      <pane ySplit="2" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L364" sqref="L364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7265625" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -56033,7 +56033,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="360" spans="1:104" s="18" customFormat="1" collapsed="1">
+    <row r="360" spans="1:104" s="18" customFormat="1" ht="15" collapsed="1" thickBot="1">
       <c r="A360" s="18">
         <v>5</v>
       </c>
@@ -56042,7 +56042,7 @@
       </c>
       <c r="Q360" s="19"/>
     </row>
-    <row r="361" spans="1:104" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="361" spans="1:104" ht="15" outlineLevel="1" thickBot="1">
       <c r="B361" s="50" t="s">
         <v>486</v>
       </c>
@@ -56094,7 +56094,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="362" spans="1:104" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="362" spans="1:104" ht="15" outlineLevel="1" thickBot="1">
       <c r="B362" s="50" t="s">
         <v>491</v>
       </c>
@@ -56148,7 +56148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="363" spans="1:104" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="363" spans="1:104" ht="15" outlineLevel="1" thickBot="1">
       <c r="B363" s="50" t="s">
         <v>495</v>
       </c>
@@ -56170,9 +56170,7 @@
       <c r="K363">
         <v>2019</v>
       </c>
-      <c r="L363" s="16">
-        <v>7.9</v>
-      </c>
+      <c r="L363" s="16"/>
       <c r="M363" s="74" t="s">
         <v>150</v>
       </c>
@@ -56202,7 +56200,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="364" spans="1:104" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="364" spans="1:104" ht="15" outlineLevel="1" thickBot="1">
       <c r="B364" s="50" t="s">
         <v>500</v>
       </c>
@@ -56224,9 +56222,7 @@
       <c r="K364">
         <v>2019</v>
       </c>
-      <c r="L364" s="16">
-        <v>7.4</v>
-      </c>
+      <c r="L364" s="16"/>
       <c r="M364" s="74" t="s">
         <v>150</v>
       </c>
@@ -56256,7 +56252,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="365" spans="1:104" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="365" spans="1:104" ht="15" outlineLevel="1" thickBot="1">
       <c r="B365" s="50" t="s">
         <v>501</v>
       </c>
@@ -56310,7 +56306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="366" spans="1:104" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="366" spans="1:104" ht="15" outlineLevel="1" thickBot="1">
       <c r="B366" s="50" t="s">
         <v>503</v>
       </c>
@@ -56364,7 +56360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="367" spans="1:104" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="367" spans="1:104" ht="15" outlineLevel="1" thickBot="1">
       <c r="B367" s="50" t="s">
         <v>504</v>
       </c>
@@ -56418,7 +56414,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="368" spans="1:104" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="368" spans="1:104" ht="15" outlineLevel="1" thickBot="1">
       <c r="B368" s="50" t="s">
         <v>504</v>
       </c>
@@ -56472,7 +56468,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="369" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="369" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B369" s="50" t="s">
         <v>504</v>
       </c>
@@ -56526,7 +56522,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="370" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="370" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B370" s="50" t="s">
         <v>504</v>
       </c>
@@ -56580,7 +56576,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="371" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="371" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B371" s="50" t="s">
         <v>507</v>
       </c>
@@ -56634,7 +56630,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="372" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="372" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B372" s="50" t="s">
         <v>508</v>
       </c>
@@ -56688,7 +56684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="373" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="373" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B373" s="50" t="s">
         <v>508</v>
       </c>
@@ -56742,7 +56738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="374" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="374" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B374" s="50" t="s">
         <v>508</v>
       </c>
@@ -56796,7 +56792,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="375" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="375" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B375" s="50" t="s">
         <v>508</v>
       </c>
@@ -56850,7 +56846,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="376" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="376" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B376" s="50" t="s">
         <v>508</v>
       </c>
@@ -56906,7 +56902,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="377" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="377" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B377" s="50" t="s">
         <v>508</v>
       </c>
@@ -56960,7 +56956,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="378" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="378" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B378" s="50" t="s">
         <v>510</v>
       </c>
@@ -57012,7 +57008,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="379" spans="2:101" ht="24.75" hidden="1" customHeight="1" outlineLevel="1" thickBot="1">
+    <row r="379" spans="2:101" ht="24.75" customHeight="1" outlineLevel="1" thickBot="1">
       <c r="B379" s="50" t="s">
         <v>513</v>
       </c>
@@ -57060,7 +57056,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="380" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="380" spans="2:101" outlineLevel="1">
       <c r="B380" s="50" t="s">
         <v>516</v>
       </c>
@@ -57106,7 +57102,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="381" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="381" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B381" s="50" t="s">
         <v>517</v>
       </c>
@@ -57158,7 +57154,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="382" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="382" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B382" s="50" t="s">
         <v>517</v>
       </c>
@@ -57210,7 +57206,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="383" spans="2:101" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="383" spans="2:101" ht="15" outlineLevel="1" thickBot="1">
       <c r="B383" s="50" t="s">
         <v>517</v>
       </c>
@@ -57262,7 +57258,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="384" spans="2:101" hidden="1" outlineLevel="1">
+    <row r="384" spans="2:101" outlineLevel="1">
       <c r="B384" s="50" t="s">
         <v>518</v>
       </c>
@@ -57316,7 +57312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="385" spans="1:104" ht="15" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="385" spans="1:104" ht="15" outlineLevel="1" thickBot="1">
       <c r="B385" s="50" t="s">
         <v>520</v>
       </c>
@@ -57354,7 +57350,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="386" spans="1:104" ht="29.5" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="386" spans="1:104" ht="29.5" outlineLevel="1" thickBot="1">
       <c r="B386" s="50" t="s">
         <v>520</v>
       </c>
@@ -57392,7 +57388,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="387" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="387" spans="1:104" outlineLevel="1">
       <c r="A387" s="110"/>
       <c r="B387" s="110" t="s">
         <v>908</v>
@@ -57520,7 +57516,7 @@
       <c r="CY387" s="110"/>
       <c r="CZ387" s="110"/>
     </row>
-    <row r="388" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="388" spans="1:104" outlineLevel="1">
       <c r="A388" s="110"/>
       <c r="B388" s="110" t="s">
         <v>908</v>
@@ -57648,7 +57644,7 @@
       <c r="CY388" s="110"/>
       <c r="CZ388" s="110"/>
     </row>
-    <row r="389" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="389" spans="1:104" outlineLevel="1">
       <c r="A389" s="110"/>
       <c r="B389" s="110" t="s">
         <v>913</v>
@@ -57778,7 +57774,7 @@
       <c r="CY389" s="110"/>
       <c r="CZ389" s="110"/>
     </row>
-    <row r="390" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="390" spans="1:104" outlineLevel="1">
       <c r="A390" s="110"/>
       <c r="B390" s="110" t="s">
         <v>912</v>
@@ -57906,7 +57902,7 @@
       <c r="CY390" s="110"/>
       <c r="CZ390" s="110"/>
     </row>
-    <row r="391" spans="1:104" hidden="1" outlineLevel="1">
+    <row r="391" spans="1:104" outlineLevel="1">
       <c r="A391" s="110"/>
       <c r="B391" s="110" t="s">
         <v>911</v>
@@ -58032,7 +58028,7 @@
       <c r="CY391" s="110"/>
       <c r="CZ391" s="110"/>
     </row>
-    <row r="392" spans="1:104" s="18" customFormat="1" collapsed="1">
+    <row r="392" spans="1:104" s="18" customFormat="1">
       <c r="A392" s="18">
         <v>6</v>
       </c>
@@ -74179,14 +74175,6 @@
     <row r="692" spans="1:25" collapsed="1"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="Y110:Z110"/>
-    <mergeCell ref="Y111:Z111"/>
-    <mergeCell ref="Y53:Z53"/>
-    <mergeCell ref="Y54:Z54"/>
-    <mergeCell ref="Y55:Z55"/>
-    <mergeCell ref="Y56:Z56"/>
-    <mergeCell ref="Y57:Z57"/>
-    <mergeCell ref="Y58:Z58"/>
     <mergeCell ref="Y126:Z126"/>
     <mergeCell ref="Y127:Z127"/>
     <mergeCell ref="AE6:AG6"/>
@@ -74203,6 +74191,14 @@
     <mergeCell ref="Y60:Z60"/>
     <mergeCell ref="Y61:Z61"/>
     <mergeCell ref="Y62:Z62"/>
+    <mergeCell ref="Y110:Z110"/>
+    <mergeCell ref="Y111:Z111"/>
+    <mergeCell ref="Y53:Z53"/>
+    <mergeCell ref="Y54:Z54"/>
+    <mergeCell ref="Y55:Z55"/>
+    <mergeCell ref="Y56:Z56"/>
+    <mergeCell ref="Y57:Z57"/>
+    <mergeCell ref="Y58:Z58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>